<commit_message>
Get daily reddit data: Tue Nov  5 08:11:05 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_10.xlsx
+++ b/data/collected_data/2024_11_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C487"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3168 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1gk1tnf</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>One thing I discovered on my nail art journey, the harder it is, the better the reward.</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk1tnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1gk0fw4</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Rate my first ever gel set</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/045xh5zm01zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1gjzm2g</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Is this a nail fail?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzxa0iy4r0zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1gjzowz</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Can you tell that I was lazy and used press on glue on my GelX tips? 🙈 Sometimes I just don’t have the patience lol, love this colour though 💙</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjzowz</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1gjzmbl</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Red and gold nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87k0izt7r0zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1gjzcsl</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Green, something new</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3sjlwm8o0zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1gjzcke</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Zebra print 💜🖤</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjzcke</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1gjzben</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkle sparkle ✨ </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6cmjhwun0zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1gjzaqr</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>New press ons 💅🏼</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjzaqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1gjyumm</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know that’s right </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjyumm</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1gjyf54</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Press on nail glue for gel x nails</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjyf54/press_on_nail_glue_for_gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1gjycjp</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Junk nails I attempted!</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjycjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1gjxcao</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do we feel about the shape and French look? </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56ufvkow30zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1gjwzhj</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Spirited Away Nails! 💜</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjwzhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1gjw3pc</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>CUTICLE CARE: How to get past anxiety/icky feeling when pushing back and trimming cuticles?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjw3pc/cuticle_care_how_to_get_past_anxietyicky_feeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1gjw3lz</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>sheer pink seeking shape suggestions</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjw3lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1gjw1gu</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I wrong for being disappointed with this set? </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjw1gu</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1gjw0vo</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>halloween nails i did</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29h9p5slrzyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1gjvysk</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Couldn’t resist the catered</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjvysk</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1gjvxs4</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">‘Nocturne’ by Mooncat. A magnetic. </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxv2yd0uqzyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1gjvjr5</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Are they cute?</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjvjr5</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1gjv95y</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Used Gelish NUDE soft gel and they won’t come off</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjv95y</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1gjv7d1</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The color that never goes out of style </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thhnknsckzyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1gjude1</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“tortoise nails” </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjude1</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1gjudxy</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do we feel about colored tips? </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfidfuuddzyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1gjud5h</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Got acrylics done at a random salon not my usual place and I really don’t like them what’s the easiest way to take them off without going to a salon that’s the least damaging</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjud5h/got_acrylics_done_at_a_random_salon_not_my_usual/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1gjtvs1</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it a bad idea to wear Dashing Diva nails to protect damaged nails? </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjtvs1/is_it_a_bad_idea_to_wear_dashing_diva_nails_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1gjtsx6</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjtsx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1gjtqon</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Kuromi Themed Nails ♡</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjtqon</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1gjto8d</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set in over two years!! </t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjto8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1gjsq9b</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Chrome over clear press ons</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjsq9b/chrome_over_clear_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1gjsxmm</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>please help me figure out a plan to strengthen natural nails</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjsxmm</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1gjt3cs</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Just wanted to use the 3D apple!</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5xeskgo2zyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1gjsk2p</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Nail lifting off nail bed under poly gel nails 😭</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9k9m7nwdyyyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1gjruos</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Calous remover</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjruos/calous_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1gjr8ga</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the best gel nail polish available? </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjr8ga/what_is_the_best_gel_nail_polish_available/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1gjquww</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Glue always peering through under my press ons</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjquww/glue_always_peering_through_under_my_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1gjqsug</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>They are still intact with three weeks of growth 😳</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3rgisimkyyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1gjqoip</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Tips for press ons?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ut9g35krjyyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1gjqfqa</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do I ask for in the salon? </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjqfqa/what_do_i_ask_for_in_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1gjqh0h</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I’m obsessed.</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq2evv88iyyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1gjqg6f</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My spring nails 🥰 do you like the length? </t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xuz3y2y1iyyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1gjqalu</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>classic french tip</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb91t2brgyyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1gjq94c</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>First gel nail extensions</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjq94c</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1gjpz69</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>is there any way to save this?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjpz69</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1gjpsmf</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Which drill bit?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjpsmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1gjoywy</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Dia de los muertos for dia de los deftones. Inspo by @ya.naily found on Google search (last pic)</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjoywy</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1gjpotb</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Which design should I pick for my next set?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjpotb</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1gjpebg</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Indian summer</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjpebg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1gjp754</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>I'm using nail wraps while some cracked nails grow out, but my cuticles are so dry!</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjp754/im_using_nail_wraps_while_some_cracked_nails_grow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1gjp330</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make my nails look less chunky?😭 </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjp330</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1gjp1j2</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finally gave up red. </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4w8x9gfq7yyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1gjosas</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just showing off one of my old sets </t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gop222bv5yyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1gjor6z</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>second set of press ons 🖤</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e3fhovxm5yyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1gjn96w</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Simple nude set 💅🏾</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjn96w</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1gjmvsp</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Halloween Nails🎃🍁</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/172js6tyrxyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1gjk5s1</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjk5s1/nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1gjkvn3</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Nail health &amp; press-ons</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjkvn3/nail_health_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1gjminz</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>My new opal nails 💕</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0go37jkapxyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1gjmhus</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Cat eye 🐱nails, even cool at night! ✨</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjmhus</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1gjmff1</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got a "bright idea" to dye my nails instead of painting them. Very unpleasant don't recommend. </t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjmff1</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1gjm6nv</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help find dupe </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjm6nv</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1gjlpfx</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>that small or would they look better on long nails? 🤔🤔</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fiev2wfejxyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1gjl0uk</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Loving the red</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjl0uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1gjkm1b</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not loving this set :( I was so excited too   The green looks like shit </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjkm1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1gjkanu</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Autumn Vibes Gel Nails</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39misj9a9xyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1gjk9v7</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>I love painting my nails white, it makes my fingers look longer and I'm in a chic and classic mood ✨😌😅✨</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/92gmjgj49xyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1gjj86j</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kuqxzkio1xyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1gjjg6v</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Tried to do an in-fill, and am thoroughly upset</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjjg6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1gjj5di</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>There's no mistake in red ♥️</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8wmf6741xyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1gjj58w</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Cool olive skin</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjj58w/cool_olive_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1gjj3p1</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>First time doing my own refills with salon- grade products. Hope you like it ☺️</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjj3p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1gj5c1y</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Gel nail damage</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2iqlbqec2tyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1gji16y</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Biab nails, how to deal with them</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gji16y/biab_nails_how_to_deal_with_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1gj4ykx</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Beginner in training. Help needed 💅🏻</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gj4ykx</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1gj8mt4</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>How do I do it faster?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gj8mt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1gjhs4t</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Tips for keeping nails healthy long-term with gel manicure?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjhs4t/tips_for_keeping_nails_healthy_longterm_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1gjhtjr</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Autumn Colours </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjhtjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1gjhscu</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>First real attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjhscu</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1gjhf93</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nails ideas? </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjhf93</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1gjhjzf</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails and how to make them last short amount of time </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjhjzf/press_on_nails_and_how_to_make_them_last_short/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1gjgncd</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flower French nails! </t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjgncd</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1gjfov6</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Colours that fit Christmas and NYE?</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjfov6/colours_that_fit_christmas_and_nye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1gjfecc</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I do for my next set?!? </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfffcfsc9wyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1gjf3g9</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Lavender Sparkle 💫</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2205edx6wyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1gjezr0</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>any hockey fans here?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfy8sni36wyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1gjern8</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Been growing my nails, what would be the best nail polish/ color or any thing to do?😁</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgs62pnd4wyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1gjcv79</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Blue Opal Crystals 💙🩵🩵🩵🩵💙</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gj92yx8nvyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1gjcrew</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Proud of the length + getting better at almond shape!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjcrew</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1gjc3rk</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Halloween set</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjc3rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1gjbwij</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>My first and second attempt at teaching myself gel nails.</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjbwij</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1gjbq9x</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Nail drill recommendations (UK)</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gjbq9x/nail_drill_recommendations_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1gjasmy</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>So happy with my new nail 🥰💅</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qxh9m6yyuyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1gj9r9h</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Midnight sky press-ons💜☁️ </t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23n42h9ckuyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1gk0mpr</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I love multichromes... but can't get them to last on me. Anyone else? Is it the brand?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gk0mpr/i_love_multichromes_but_cant_get_them_to_last_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1gk0jjs</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Blue Valentine💙</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk0jjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1gjzzss</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>First Emily de Molly order!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjzzss</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1gjzo9d</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Polish the color of this lollipop!!</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/274udxkrr0zd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1gjzk4x</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Hoping on the blue train!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjzk4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1gjzgvy</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue blue blue 💙 </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjzgvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1gjydz5</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>I voted early but still ready for tomorrow</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjydz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1gjy2pg</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>VOTE 💅</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/595ro8z4b0zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1gjy2hx</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Similar color to Sally Hansen Color Therapy, One Day At A Time</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjy2hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1gjxfv5</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Shape-shifting in the Moor</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f2e7ld6v40zd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1gjxb9s</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>If you’re still looking for a dupe for Polished for Days Goblins and Ghoulies, this LynB Mishipeshu is awesome</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjxb9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1gjvw6f</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Why Do My Topcoats ALWAYS Shrink?! 😭</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvg8r5fgqzyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1gjvrur</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Admiring the shift in my nails at work 😆</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1a7idoepzyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1gjvh9e</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Cirque- worth it?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3nt78ismzyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1gjupa9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Monarch - Psycho</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjupa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1gju4nb</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Cozy milk tea nails for fall!!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gju4nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1gjtyj2</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Morgan Taylor Sunrise and the City</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjtyj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1gjtwba</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First thermal polish and first time having long nails = obsessed (fancy gloss mango dulce) </t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t5xbuia9zyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1gjtkwd</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Nail polish made of gems is an ingenious idea</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjtkwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1gjt14t</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Super short rescue manicure</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l7dqm562zyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1gjswvf</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Dupe for Cirque colors witching hour?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjswvf/dupe_for_cirque_colors_witching_hour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1gjsqmz</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Blue Election Day Mani </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/letz61muzyyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1gjsbgc</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>I made Nail Polish 🤯</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjsbgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1gjr5l4</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>So impressed with this orange</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjr5l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1gjq6yh</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>❤️Ready to rumble❤️</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjq6yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1gjq3sv</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>No no, I’m ✨obsessed✨</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjq3sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1gjpw84</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>🍂🍁🦃</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjpw84</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1gjpi6k</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>It’s giving… Christmas? 🌲🌟</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fj3fb9k2byyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1gjpc66</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>a moment for the nails</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv0zseiu9yyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1gjoztg</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>I may have a problem</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71oazkid7yyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1gjorp4</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Happy (Almost) Election Day!! 🇺🇸</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/v5mrl4p.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1gjoqcx</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Glam green…</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqnd8fvg5yyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1gjokto</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flakie bomb finger dance ft. Swamp Gloss &amp; Pahlish </t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjokto/flakie_bomb_finger_dance_ft_swamp_gloss_pahlish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1gjo4ja</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This sub inspired me to wear CG Afterglow for my wedding! </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0atkihb01yyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1gjnw1f</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Comparison of Polished For Days “Quite Literally Dead Inside” (Sept. ‘24 PPU) &amp; KBShimmer “Dead Ringer” (Fall 2024 collection)</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjnw1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1gjnvme</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>help finding a color!!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjnvme</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1gjnr51</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Death Valley - Marigold and Wildflowers</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjnr51</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1gjnk9b</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat - Queen of the Dead </t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjnk9b/mooncat_queen_of_the_dead/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1gjnj07</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whiskey Sunrise </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjnj07</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1gjn9tx</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Almost the day!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/308xhunuuxyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1gjn4i9</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Darkest Hour 🌚</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjn4i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1gjmjgb</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Fixing my nails.</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xp6mrjgpxyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1gjktbe</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Intense bioluminescence is right 💙</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjktbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1gjkowd</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Chocolate nails to welcome in November 🍪</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjkowd</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1gjkgxf</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>My chickens be chickening - showing off my Fierce Mojo from Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjkgxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1gjka29</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Hello from Washington DC 💀</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjka29</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1gjk4qf</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>To the person who mentioned you need to dab your cleanup brush before you use it to remove excess acetone…thank you!</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t98xe8r38xyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1gjjvyh</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These 3d printed magnet holders are a game changer! </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjjvyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1gjjvsx</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rosalie </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjjvsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1gjjuxw</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>LynB issues automatic refunds</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjjuxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1gjjjyl</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>What shape are her acrylics?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gzzjck14xyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1gjjb9r</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t xml:space="preserve">purple blue gradient from cirque jellies! </t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzng3owa2xyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1gjj29g</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At-Home Hypoallergenic Gel? </t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjj29g/athome_hypoallergenic_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1gjj0r8</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Probably the prettiest multichrome ever. 😍</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjj0r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1gjiz1m</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I gave in. Are you happy now 🥲 </t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4b98pbxvzwyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1gjivvx</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Dupes for this shade? 😩</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvhjjas8zwyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1gjipkg</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Always makes me think of root beer 🍺</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcczkvm0ywyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1gjicty</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>ILNP - Honeymoon</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivny3o7fvwyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1gji4ha</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Myself am Strange and Unusual </t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gji4ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1gjhe3s</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I pls get a moment of silence 😭 </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjhe3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1gjh4oy</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Vampire Nails All Year Round</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjh4oy</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1gjh3py</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>It’s time.</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9tj3cxwamwyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1gjgo5y</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Accidental Skittle</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjgo5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1gjgk6t</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>All ready to downvote blue!!!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2az9gz06iwyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1gjfb7d</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amazon Hub/USPS Packages </t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjfb7d/amazon_hubusps_packages/</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1gjex9v</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I found my holy grail base coat! </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjex9v/i_found_my_holy_grail_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1gjdd7t</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Magnetic nail polish - how do you work one nail at a time?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjdd7t/magnetic_nail_polish_how_do_you_work_one_nail_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1gjc1f0</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Dark Heart - By Dany Vianna</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjc1f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1gjbm76</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjbm76/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1gjbhkn</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do I get better pictures of my nails when I'm not even trying to photograph my nails? </t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvu3zof08vyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1gj9w9b</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Thank you for the tips!</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl2ikj1cmuyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1gj9s9c</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Duble the base coat, they said. It will protect you from staining, they said.</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gj9s9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1gk1n6n</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Random nail art I ended up liking</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk1n6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1gk1jyq</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Never done this style before</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk1jyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1gjzg3t</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kkxkbubp0zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1gjy4kg</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend painted my nails to match my cats eyes! </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjy4kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1gjw97x</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Midnight Marg🍹</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/caxr67sntzyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1gjvj62</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>nail art tips?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gjvj62/nail_art_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1gju7iz</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>My newest set</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gju7iz</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1gjquux</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Nail teeth 🦷</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjquux</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1gjostm</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Little dinos</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/412v3g8z5yyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1gjno8n</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>my nail tech ate [she is not a professional]</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjno8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1gjn109</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not perfect, but I like them </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjn109</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1gjme1d</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hands were so shaky! But I'm proud of my little stars. </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjme1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1gjm97g</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>my god, I think these are the most beautiful nails I've ever had done.</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yvokuhhdnxyd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1gjm1y6</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Love the blue and dot glitters</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jjx019zlxyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1gjhcu7</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Royal blue and white nails 💙</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjhcu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1gjdvzr</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ok 2nd attempt! </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3kmjy5uwvyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1gjd09f</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Fascinated with the color pink! 🩷</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7sleigzlovyd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1gjc4ge</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>I'm happy they look beautiful 😍</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/temivziefvyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1gjbfgm</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clay Doh rises anyone </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjbfgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1gjbabj</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recreation of a Tino Vo design. </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sm33lbc5vyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Nov  6 08:10:59 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_10.xlsx
+++ b/data/collected_data/2024_11_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C487"/>
+  <dimension ref="A1:C696"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8712,6 +8712,3559 @@
         </is>
       </c>
     </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1gktc81</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>New nails! Finally getting some length again 💜</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gktc81</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1gksr70</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Somebody reported my previous post with my manicure, which had the othala symbol (ᛟ)</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gksr70/somebody_reported_my_previous_post_with_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1gkry81</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>frenchies + buildergel on my natural nails !</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkry81</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1gkrfne</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>I fixed my nails! Before pictures at the end for those who haven't seen.</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkrfne</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1gkqmxf</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkqmxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1gkqhj5</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tried gel x for the first time </t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkqhj5/tried_gel_x_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1gkqh3z</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Experimenting with colors 🌈😊</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/caepu968o7zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1gkpcss</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Learning About Gel Nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkpcss/learning_about_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1gkp4c5</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving all the fall colors with this mani 🍁 🍂 </t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ou7h1aq97zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1gkowl9</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Super curious how much is everyone paying to get their nails done?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkowl9/super_curious_how_much_is_everyone_paying_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1gknm3n</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>yellow nails.. yay or nay ? 💛</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ls8xlq2pu6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1gknkae</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Beginner</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gknkae</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1gkn8nz</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>received mixed opinions on this set irl</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkn8nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1gkmytr</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>SNS color change?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkmytr/sns_color_change/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1gkmz3b</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>discontinued Essie color "tropic low"</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkmz3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1gkmyi3</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn nails 🍂 </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ygbp8wdo6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1gkm2hr</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Gel clumping ?</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5b9hev87g6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1gkmjw5</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>First Christmas set done! First time using sculpting gel and it was so fun! I've already got another idea in mind and I can't wait!</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o45ibfsjk6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1gkmijd</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This month’s nails. Dip manicure. </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkmijd</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1gkmeu9</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your favorite magnetic (non-gel) polish brands? </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkmeu9/what_are_your_favorite_magnetic_nongel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1gkm4oo</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new nails ! </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkm4oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1gkljqd</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Press on recommendation for wide nails</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkljqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1gklgyp</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>My Golden claws ⚜️11 month growth 😻I can’t get over stilettos 🔥</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gklgyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1gkkwyk</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Using my dotting tool for the first time </t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fatcrp4f66zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1gkkpau</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Am I too rough for acrylics?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkkpau</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1gkk6wg</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some recent-ish nail designs i’ve done! all are hand painted </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkk6wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1gkjx92</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Toenail clippers for thick nails?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkjx92/toenail_clippers_for_thick_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1gkj23s</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Remember to organize your supplies!</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkj23s</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1gkj0c8</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Tip snapped off.. stumped on what to do now. Can I just glue it back on? 😅</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqnstb9yq5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1gkivsu</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>New Set 🤩</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdlohjbzp5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1gkisyi</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Streaky nails</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkisyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1gkiqni</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>New Set 🤩</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vv7lv8two5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1gkicqe</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>new nails for fall🍂</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5w1obtyl5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1gkhxfu</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>My cuticles ruin everything!</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkhxfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1gkgxzc</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail edges (white part) goes low and there’s these marks from gel powder that doesn’t seem to go away </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zs5c1oz8b5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1gkhpb8</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Did it for a pumpkin farm festival. Forgot to post</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fcgsy2yg5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1gkhipw</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>You like?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6tn9v2nf5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1gkh7si</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Dupe for OPI Bubble Bath?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkh7si/dupe_for_opi_bubble_bath/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1gkh28y</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>😊🥰</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ussaw137c5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1gkh1vh</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>💖💖💖</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pqcnq8j1c5zd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1gkh1e4</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Art liner gel recommendations </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkh1e4/nail_art_liner_gel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1gkgrjw</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>It's the prettiest red</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkgrjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1gkgdgc</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Weirdly enough my right hand  turned out better, it is usually the worse one</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkgdgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1gkg2qp</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Another one of my favorites</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mz1va8d45zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1gkfzn3</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else watch Not So Pretty on HBO Max? It covers hair, skin, makeup, and nail industry. It’s a 4 part series </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7xieivz35zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1gkfdyi</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X Extension with Cat Eye </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyzzcz2hz4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1gkf3gd</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh press-on set from Ulta </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mdx26f9x4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1gkdk3d</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My election nails inspired by Beyonce but not executed as well as hers. </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98qpdyqyl4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1gke85q</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done </t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9qumcqztq4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1gkdzik</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>What kind of chrome would achieve this look?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vknuz4g1p4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1gkda5v</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Is this from poor application?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkda5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1gkd0vc</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Sally Hansen 'Limelight'</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvg3sr2yh4zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1gkcdnm</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying semi cured gel strips </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dsrfrw5d4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1gkc3ca</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Acrylic over gel?!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkc3ca/acrylic_over_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1gkbybw</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Fall nails 🍁🍂🧡</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkbybw</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1gkbn1c</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to recover mi nails. </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkbn1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1gkbf0x</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>New fall season nails have dropped!🍃</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkbf0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1gkaxpc</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Recommendations for High Gloss Top Coat</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkaxpc/recommendations_for_high_gloss_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1gkapnq</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Clear Polish</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkapnq/clear_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1gkakvh</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>They are growing little by little ❤️‍🩹</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu7uqdcsz3zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1gkajxs</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the reason for cuticle cutting/pushing back? </t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkajxs/what_is_the_reason_for_cuticle_cuttingpushing_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1gkaiy2</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Ersa nails</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkaiy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1gka1xs</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>What did my nail tech put on me and how do I get it off?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gka1xs/what_did_my_nail_tech_put_on_me_and_how_do_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1gkabwv</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>My natural nails</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkabwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1gka7at</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>red + gold = ♥️✨</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqu4q9czw3zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1gk9u5b</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tv8aho7u3zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1gk8yc7</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>💕💕💕</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3a9kusjen3zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1gk2pmp</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Help, my nails are constantly peeling/breaking! :(</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk2pmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1gk8fm3</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I use clear press ons like nail tips? </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gk8fm3/can_i_use_clear_press_ons_like_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1gk3k2o</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>How I achieved this</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk3k2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1gk8s66</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>NEW NAILS 🔥🔥</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk8s66</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1gk852y</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>She did it againnn 😍</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk852y</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1gk7s3v</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Fall = Purple 🍁</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9p7hyawd3zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1gk7q3y</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Ready for my vacation 🌸 what do you guys think?🥰</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hd4g2kgd3zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1gk7n8q</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>YN professional gel kit</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gk7n8q/yn_professional_gel_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1gk7ku5</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vacation Mani! (Natural Nails) </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk7ku5</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1gk76ei</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My second go at almond shaping </t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk76ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1gk6v2z</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u6uz6pe63zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1gk6u8l</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Set I did </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk6u8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1gk67im</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">La francesita, a classic that never fails </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnu3gpoh03zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1gk64p5</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just can’t stop getting red! </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk64p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1gk5j7e</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>If you’re in the US and eligible - don’t forget to vote</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvi8p415u2zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1gk4kto</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Wednesday and Enid UV Nail Stickers by Maniko</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk4kto</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1gk410r</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>First attempt at the vampire nail trend</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/il0t6a26d2zd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1gk410k</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Halloween nails 💅 </t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lawp7zz5d2zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1gk3cli</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>My first set!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1onbgvc42zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1gk2kv2</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Cat eye Blue with black. I think it’s time for a new set.</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0434rowjt1zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1gkk2w0</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>When you vote blue but your polish is pink.</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkk2w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1gktgjq</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Dupe for OPI Yoga-ta Get This Blue</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzr2jff5n8zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1gksu75</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Blu Tack and a false nail</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gksu75/blu_tack_and_a_false_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1gkqw4c</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hi! Looking for a polish (no gel/curing) that is similar to this color (berry red for fall). Ideally it would have a bit of that transparent crelly look to it but straight cremes are fine too. Drugstore recs are preferred. </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w25qaivqs7zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1gkqt7h</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Indie advent calendar?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkqt7h/indie_advent_calendar/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1gko8nr</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Voted early, mani'd late!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fwrjxmp07zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1gknxi9</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>🩵💙Blue Gradient💙🩵</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gknxi9</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1gknsxj</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Did I paint over an existing mani quickly this morning for reasons? Perhaps.</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2ufbmegw6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1gknq8t</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>helping to spread the BLUE vibes 💙</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fgwrbgrv6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1gknh5w</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>A fun blue for the occasion!</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gknh5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1gkngq1</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Mani-festing with you guys 💙</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d13fb6f8t6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1gknd5f</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Best blue I had</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhzdv0h9s6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1gkmyi0</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Joining the blue wave 🌊</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkmyi0</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1gkmve3</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>I can’t stop staring at my nails ✨💿🌈</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3kpnpwckn6zd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1gkmtm7</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Joining the Blue Crew</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkmtm7</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1gkmond</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>I bind you…</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkmond</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1gkmlsg</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Cornflower Blue</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg22s1t1l6zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1gkmkql</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>I'm loving all the blues today</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9e1ep2amk6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1gkmeut</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Vote</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzjv1snaj6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1gkmbxt</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>My 1st vote</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkmbxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1gkm4t1</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Mixed Berries</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkm4t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1gkllab</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue or I’m begging for an abduction 👽 </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rlyhr0l1c6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1gkleki</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to manifest some good juju tonight! </t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkleki</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1gkl3ku</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No blue polish? No problem! </t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkl3ku</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1gkkppi</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>I think I understood the assignment…</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkkppi</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1gkkmnw</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Manifestation Mani on Election Day</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjp6pob146zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1gkkmmg</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Nails of the Day</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs12stt046zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1gkkhmb</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Voted! Then went to the library </t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkkhmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1gkkg95</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Second Time Doing Gel</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkkg95</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1gkkb9v</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Just voted from Michigan and joining the blue wall 💙</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pxmwqsd16zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1gkk1uq</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>I was so excited to join in today!</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijn9kb3az5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1gkju5k</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>A badly broken nail won't stop me from having 5 matching fingers</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28m3savix5zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1gkjpz7</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>💙🌊 Let's goooo!</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo4m4f2lw5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1gkjpa1</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Sally Hansen insta dri-tips dried matte?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkjpa1</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1gkjijb</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Kamala Blue from Australia 🇦🇺 only blue I had - Chirality "the night before". Good luck everyone in the States today, stay beautiful and stay safe</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpcrwkbxu5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1gkjay2</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Heard we're doing blue today </t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kusfju4t5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1gkj7ig</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>so utterly in love with this colour that isn't made anymore 😭</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkj7ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1gkj3u0</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Thought about joining the House of Harris (Hades) hype train but...</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcagbxrpr5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1gkj2ua</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Had a red/black multichrome polish on from Halloween but had to do a fresh mani-fest to go vote 💙</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqzgobchr5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1gkiqe2</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Help please. Cracked nail emergency.</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkiqe2/help_please_cracked_nail_emergency/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1gkipoo</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Took a half day</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2puu43po5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1gkinjf</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>🌊🌊🌊</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l89mk2o7o5zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1gkikz6</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>First time voter 💙💙💙</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkikz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1gki93d</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>ISO stamping plate</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gki93d/iso_stamping_plate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1gki4eo</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>A sparkly fall mani</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8obxgz6k5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1gki2fv</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Mojave Dreams</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gki2fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1gki1eg</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>In honor of you, Marie 💙🦋</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbuq0esjj5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1gkhwf8</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bengal kitty nails 🐾 </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ecy31rhi5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1gkhvwz</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue Skittle for Today </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkhvwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1gkhtls</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Blue dot in a red state</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkhtls</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1gkhr08</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>First Magnetic Mani, tips???</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkhr08/first_magnetic_mani_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1gkhqfc</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another 🤞💙💅 </t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bg7jd0f8h5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1gkhlth</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chose the early campaign color because voting is brat. </t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgqpnfjag5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1gkhks3</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving all the blue manis today💙 </t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e40jbmf2g5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1gkhiwu</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Red Nails For Today ❤️</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkhiwu/red_nails_for_today/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1gkhh6j</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>My mother-in-law asked for "a Kamala Manicure" and I was happy to help her out! She has good taste!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k5nkau0f5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1gkhh6c</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Had this super unique and original idea to paint my nails blue today</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkhh6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1gkhdn9</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Blue blue blue</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h41971tke5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1gkh5n7</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Salon application of builder gel a question</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkh5n7/salon_application_of_builder_gel_a_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1gkgtje</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Nail salon applied builder gel and it was very painful —why?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkgtje/nail_salon_applied_builder_gel_and_it_was_very/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1gkgyo9</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I hear we're posting our lucky blue manis today </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkgyo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1gjwzmc</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>What is a random thing that kills your manicure?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gjwzmc/what_is_a_random_thing_that_kills_your_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1gjxobr</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Top Coat Question</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gjxobr</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1gkgumj</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can anyone recommend a color that matches these sexy Ferraris? </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/008rgwfja5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1gkgtsm</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Progress - 2 years of lazy polish/manis</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l01gfoaa5zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1gka3me</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>heptane thinner with thermal polishes?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gka3me/heptane_thinner_with_thermal_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1gkf128</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Daveen Swatches Love!</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkf128</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1gkgp09</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Galaxy gray dupe?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkgp09</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1gkgnyj</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>💙🩵Manifesting with my mani 💙🩵</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkgnyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1gkgid9</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue Crew! 🌊📝📥🌊 </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkgid9</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1gkghs3</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat lady nails </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayieadkt75zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1gkg2c6</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>LET'S GO</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xaem7dtk45zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1gkfwdq</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Decision 2024 inspired manicure ❤️🤍💙</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkfwdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1gkfssv</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joining the sea of blue manis today 💙 </t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kghygzol25zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1gkfpd8</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Another one</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cpol85w15zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1gkfjmh</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Varnish chips and takes away layers of my nails with it 🥲 how do I avoid this? </t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkfjmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1gkfbr9</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">😰 nervous </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkfbr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1gkf22c</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Midnight kiss ILNP (blue wave mani)</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2pvzo3zw4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1gker8a</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vote vote vote! </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gker8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1gkekfe</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>10 months... gone in a flash 😭</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkekfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1gkeie8</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>ILNP Shooting Star for good luck ✨</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkeie8/ilnp_shooting_star_for_good_luck/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1gkei56</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>As a reformed nail biter, this is the longest and shapeliest my nails have ever been 🥺 (and my first thermal—so fun!)</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rl7508ks4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1gkeffl</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Nail polish thinners for base and top coats?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkeffl/nail_polish_thinners_for_base_and_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1gkeb1d</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>It's very time consuming to do magnetics ft. Phoenix Mistress</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkeb1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1gkeawj</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grave Consequences Indeed </t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goyzjs9cr4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1gke136</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Let’s go! 💙</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ruf80cdp4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1gkdqnf</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Kamalaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyk4k2m8n4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1gkdnpt</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Joining the chorus</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lm0008znm4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1gkdlw8</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feral Gremlin Energy for today’s election. Vote like your life depends on it because it does. </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkdlw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1gkdd2c</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Lurid Black Friday sale?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkdd2c/lurid_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1gkcymd</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Let's Go!!! 🌊</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkcymd</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1gkcg7f</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Those Blue Memories</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkcg7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1gkceue</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need OPI recommendation </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkceue</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1gkcdnp</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I always wear blue, but I understood the assignment! </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epxs3b16d4zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1gkc83e</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>I had a red nail polish I really wanted to try, but simply could not because of today. My partner said, “Who cares?” All of these blue manis make me feel vindicated!</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gkc83e/i_had_a_red_nail_polish_i_really_wanted_to_try/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1gkbxdf</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Manifesting positivity for a brighter, better, and stronger tomorrow 🇺🇸☑️💙</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k782wys94zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1gkbvyr</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Voted For Human Rights!</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkbvyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1gkbl5b</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>💙💙💙</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkbl5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1gkbj1m</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Voted in Pa, trying to manifest a blue wave🥹</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkbj1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1gkbg1u</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Heading into today trying to be calm and hopeful</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkbg1u</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1gkt56o</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I asked for vs What I got </t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cxv8ct7j8zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1gkp0c8</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amateur nail art loosely inspired by khokhloma </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkp0c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1gko6tu</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Omg 😱 I love this nails. What do you think ?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etjumi5b07zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1gknp6q</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>These rhinestone shapes are so perfect for Christmas 🤤✨</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iv85nlhhv6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1gkmzrg</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>I love my nails this week!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5gpuzmpo6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1gkmirf</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>First Christmas set done! First time using sculpting gel and it was so fun! I've already got another idea in mind and I can't wait!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffxmo0e9k6zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1gkky11</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Blue goes well with everything</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6m8ii9j66zd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1gkkvpv</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Just done dots. Lol</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9na68w366zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1gkjy28</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Too much polish when marbling</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/si0wumxfy5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1gkjx4o</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Manifesting some good juju tonight! 🔵</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkjx4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1gkj6n4</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Nails I did on my sister🥰 insta @hair.with.drew</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nuvbjzbs5zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1gki82d</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wip commission </t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gki82d</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1gkfpgr</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am a beginner </t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/349c71ex15zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1gkfdxd</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it giving pinstriping or lowrider or nah </t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkfdxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1gkeerd</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Funky fall nails hand painted on myself 💅🏼</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkeerd</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1gkc4iy</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Sailor Neptune Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkc4iy</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1gkb3z1</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Art liner gel recommendations </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gkb3z1/nail_art_liner_gel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1gk95dd</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Birthday Nails!</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk95dd</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1gk75mh</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I love my pink acrylic nails</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpaixsou83zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1gk6r75</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My newest set (and maybe fav) </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk6r75</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1gk6kgp</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pennywise nails! </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gk6kgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1gk5an5</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>My chosen color for the beginning of this month 🤗</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3vh67zor2zd1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Nov  7 08:10:37 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_10.xlsx
+++ b/data/collected_data/2024_11_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C696"/>
+  <dimension ref="A1:C862"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12265,6 +12265,2828 @@
         </is>
       </c>
     </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1gllacz</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got my nails done today and I’m obsessed 🤩💕✨ </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jzuwxvf3pfzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1glkw5a</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Hi guys, I just did black for the first time with my natural nails, I'm trying if it'll go with bold colors😁 I'm going to try jelly pink soon 🩷</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mw7i1ehmjfzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1glkpdt</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Got a new nail set of acrylic overlay on my natural nails. Plum nails💜🪻🍇</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8fn99o8hfzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1glk988</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Rainbow chrome dreams🌈✨</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glk988</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1gljhjt</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>New set finished 💅🏻</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qvjab0n2fzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1gljg5q</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Changed my set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cawdxb72fzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1glj19m</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Morbidmegannails on insta. Has anyone ever seen an American traditional nail set?!?! 😍</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0a9gx3nlxezd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1gljdqs</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Polygel vs press on</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gljdqs/polygel_vs_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1glj4m7</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glj4m7/new_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1glinvo</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>UV Lamp - Itchy fingers</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glinvo/uv_lamp_itchy_fingers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1glfl6y</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>My mani and my dog, two things that brightened my day. Mani inspired by tessa.lyn.nails on IG</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glfl6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1glh1tp</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>I recent started doing dip nails, can i refill instead of starting from scratch?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glh1tp/i_recent_started_doing_dip_nails_can_i_refill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1gli11t</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Please help me choose a colour.</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxr1cyp5nezd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1glhz3n</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting black on nails. What color for toes? </t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glhz3n/getting_black_on_nails_what_color_for_toes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1glhxm1</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>acrylic fill vs gel Polish</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwep82i6mezd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1glhn8p</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">business name ideas </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glhn8p/business_name_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1glh9d4</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Camellia</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glh9d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1glh82t</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Christmas gift for "adopted" teen?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glh82t/christmas_gift_for_adopted_teen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1glh2ul</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Recommendations for new nail lady in Miami?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glh2ul/recommendations_for_new_nail_lady_in_miami/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1glh0t4</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>My favorite set I've done yet! 💅🏼</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glh0t4</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1glfsaa</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>should i get a gel manicure</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glfsaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1glgz1g</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>THERMAL NAIL POLISH 🩷💙</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glgz1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1glgclb</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished painting the AHS logo for my nail set! 🥰 </t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlsaczxl6ezd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1glg52u</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Cow Nails!</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21os2dqo4ezd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1glfgy8</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Nail time!</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3xznmqkydzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1glfe16</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Lazy fall</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glfe16</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1glf8xx</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Wholesale Suppliers</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glf8xx/wholesale_suppliers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1glf4ey</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growth progress :) </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glf4ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1gldsm5</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Realized today that I have weird ass hands, but I love this set!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbg2kldzjdzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1glehjf</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Glitter nails—switched to acrylic from dip 😅</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glehjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1glefw0</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Not everyone’s cup of tea but I really worked hard on this set</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glefw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1gle6vd</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Maybe one of the coolest manicures I've done</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/svzz8498ndzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1gldtzn</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Set Red </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nbrvazakdzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1gldmp4</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Advice needed for a beginner.</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gldmp4/advice_needed_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1glcqu9</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Did I overpay for these?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glcqu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1gld5cs</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Builder gel won’t come off!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gld5cs/builder_gel_wont_come_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1gld2sj</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Color?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/da68e7u1edzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1glcwky</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vjil1jkcdzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1glcllm</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Looking for Tips on Getting a Thinner Nail</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glcllm</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1glcjau</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>So…what now?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns67vrak9dzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1glccl5</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Gel polish at home</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glccl5/gel_polish_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1glc0vv</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Damn you, metal nail file</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50s1dmxd5dzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1glbr2c</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Which of my nail designs is your favorite?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glbr2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1glbdaj</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am obsessed </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd7asge80dzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1glam5e</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Obsessed with my new set!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glam5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1gla8d4</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any love for some short nails? </t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gla8d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1gla2g2</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>My first REAL fake nails!!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4zh1ri8qczd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1gl9cb1</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Going on a magician themed cruise on Saturday. </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2e1midqkczd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1gl9516</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>recent e-file+diamond bit cuticle detailing x structured manicures x hard gel nails I’ve done on my clients 💘</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl9516</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1gl8tkp</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Do you like them sharp?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vv9t9rtgczd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1gl8iru</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>New set 😍💜</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl8iru</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1gl6r55</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>I love the way the flames burn</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nxeikinf1czd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1gl5mbg</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Why do my nails peel away like this after I paint my nails? I use a base coat and a top coat. (Don’t mind my horrendous cuticles..)</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl5mbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1gl05g0</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Help me with shape.</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqu9vg4hnazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1gl4kw0</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>SOS!! Need help deciding on vacation nails!!🏝️</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl4kw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1gl4yom</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Thermal lacquer!</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f00c6g5obzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1gl72he</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Care after soft gel nail extensions removal?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gl72he/care_after_soft_gel_nail_extensions_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1gl778d</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Hi there! I am looking for this gel shade in DnD, OPI or CND. Thanks in advance!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkbxy82q4czd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1gl6y1w</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Left thumb nail is stickey after gel mani???Feels dry and fully cured, but like adhesive rubbed off on it. Noticed it before I touched anything and won't wash off. </t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl6y1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1gl6qqw</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Any recommendations for the colors in the picture? I‘m new to the nail game 💅💕</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ifw3vnpc1czd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1gl64bx</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>gel chips after a week?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a39ln17qwbzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1gl5rco</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Nails I’ve gotten 😋</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl5rco</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1gl5fj1</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Some clean coffin nails</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl5fj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1gl57ti</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Throwback to when I took my fiancee to get her nails done and decided to have mine done cause I was bored. </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xil03vt1qbzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1gkyot7</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Is there any way to have long nails without ruining my actual nails?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkyot7/is_there_any_way_to_have_long_nails_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1gl4iiv</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>My (pre)winter nails</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl4iiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1gl3ee6</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>It's like I'm wearing... Nothing at all 🍑</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xc73zvvgcbzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1gl2rpv</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Obsessed with my gold frenchies😍</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aotkllxs7bzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1gl2q4e</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Burning Desire </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsmhvn4i7bzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1gl2j8v</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1ot9a206bzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1gl2hwu</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new set on my natural nails 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl2hwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1gl27q1</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Wait shape and length for my nails?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzsj8ujk3bzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1gl27nh</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Stick Season gold set done by me</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/dsEQU5o.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1gl1mn6</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">polish recs? </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gl1mn6/polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1gl1gqd</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Got my nails done on Monday morning</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy7bkjhsxazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1gl1g1z</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Unusual fall nails @isabelfreitasnails</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl1g1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1gkzaz8</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Glass File Does Not Seem To Work?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkzaz8/glass_file_does_not_seem_to_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1gl0xpl</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>French tips with a twist 😍</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j83rofwltazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1gl0w57</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">THE tragedy </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl0w57</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1gl0qar</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>I paid $100 for my girl to get her nails did but she doesn't like them because she can see her old nails. Can yall tell me where the nail tech screwed up?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cv201s71sazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1gl0e6e</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Press ons i’ve made for fall so far</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl0e6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1gkzxve</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Wineberry</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkzxve</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1gkzr71</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Vampire nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkzr71</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1gkzkmh</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Fall nails I did</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyp3sjioiazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1gkzhx5</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glittergel for The dark season </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omn7i873iazd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1gkz96r</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Luckily I'm doing my nails tomorrow. </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v1g4xznfazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1gkz02g</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>🫶🏻</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dd1sn7vxdazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1gkyaez</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>This time I decided to do a simple plain manicure</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkyaez</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1gkvlaz</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Washing hair after acrylics? </t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gkvlaz/washing_hair_after_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1gllhh5</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Essie sugar daddy swatch on 128 warm nude</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdi3wl405gyd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1glkc8l</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Closest non-gel equivalent?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glkc8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1gljhrv</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>nail art</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gljhrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1gljdjs</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>My mourning of democracy mani</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtjm30ce1fzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1gli05q</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grieving </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeynm2pwmezd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1glhsne</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Glow in the Dark Birthday Nails 💚💡🥳</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glhsne</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1glhqww</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Just gotta keep sparkling on ✨️💙✌️</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glhqww</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1glgr06</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Fiending for a black nail polish that has a quick dry time</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glgr06/fiending_for_a_black_nail_polish_that_has_a_quick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1glg8dr</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FIRST THERMAL OMG </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glg8dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1glfxq6</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Seche vive + Cirque</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glfxq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1glfsa6</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Protesting the election results by wearing Mooncat’s Petals for a Narcissist. Seemed fitting. </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dl5k952f1ezd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1glfhah</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>thank you to this sub for introducing me to seche vite</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glfhah</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1glfbz7</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An Unshakeable Sense of Foreboding... For reasons. </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl27h8ucxdzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1gldxly</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Well, if that isn't a fitting end for today</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0oovpq5ldzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1gldxip</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Cranberry for fall 🍁 </t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gldxip</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1gldhit</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>At least we still have nail polish….</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gldhit</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1gld7x0</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>I bought the entire OPI x WICKED collection (part 1)</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gld7av</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1glc8ac</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupes for this shade/look?? </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glc8ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1glc4gy</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Have you ever 'burned' your nails?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glc4gy/have_you_ever_burned_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1glbubb</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Firey Mani on this cold snowy day 🌨️❄️</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glbubb</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1glb7gf</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>What are these “splinters” on my nails and how to deal?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glb7gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1glazon</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Quite Literally Dead Inside </t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glazon</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1glaxsq</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>The only color I thought would be appropriate for today 🏴‍☠️</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyw1dnrvwczd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1glavk9</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Thank you all 💙🖤🩶💚💜</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glavk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1glaf4u</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some Cat+Nails! </t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glaf4u</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1gla6cs</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>My 1st PPU</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gla6cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1gla5zt</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Some OPI blues</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t9ey4vlyqczd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1gla4gi</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Idc im keeping my blue mani 🥲</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gla4gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1gla3ly</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Name of this color is too on the nose - Bottled Rage</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8dmwnfhqczd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1gl9mwp</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Magnetic lovers looking for retail therapy this week: Clionadh just announced a Psilocybin inspired mini collection</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl9mwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1gl9dsc</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>If voting didn't get us there, we fight for the world we want to see.</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynrmxwp0lczd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1gl973g</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>I promise they're not red for the reason you think</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl973g</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1gl939d</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Sick to my stomache, so i redid my nails💅💗⚰️</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl939d</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1gl902a</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Can’t decide between Cirque Colors Mood Ring or Mooncat Serpents of Eden</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gl902a/cant_decide_between_cirque_colors_mood_ring_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1gl8q9a</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I wanted to mani-fest a sane outcome but here we are... Feels like a punch in the gut but at least my nails look cool... </t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl8q9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1gl8dbj</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>We'll get through this. 🩵</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl8dbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1gl7nwt</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Good news: Peely base working as expected</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3o1tbo38czd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1gl7474</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My hit of dopamine in these trying times </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl7474</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1gl72p2</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dazzle Dry Mojave Dreams. The difference direct and indirect light makes </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl72p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1gl6hyg</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Decided to recreate my first mani ever for no reason in particular</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl6hyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1gl6750</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Extremely disheartened about today and what the future holds for Americans. This was supposed to be an autumnal gradient, but I want it to represent the fire in my heart right now. </t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl6750</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1gl63ef</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>hearts unite. 💕✨</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/miigthbjwbzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1gl5s8q</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t know if this is the place </t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl5s8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1gl5l17</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mourning mani </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lasads9rsbzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1gl5hiz</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>At least I can admire my pretty nails to disassociate from real life 🥲</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1baumud0sbzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1gl3amu</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Indie polish convert </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl3amu</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1gl52qu</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Reached my length goal! Never thought my nails could look like this</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl52qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1gl4pm8</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Some pink holo for hope.</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it64q480mbzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1gl4gxn</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>To lift the mood</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl4gxn</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1gl41vm</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Watery polish wwyd</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gl41vm/watery_polish_wwyd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1gl3jft</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>mixing polish (regular + gel)</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gl3jft/mixing_polish_regular_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1gl370e</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Best topcoat if my priorities are shine and no chips</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gl370e/best_topcoat_if_my_priorities_are_shine_and_no/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1gl2ovn</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Red For Today ❤️</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofljrbl87bzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1gl2j8k</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Scrolling through all the blue manis from yesterday really adds to the gut punch</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9lc4fxz5bzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1gkyxvm</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Milky calm white</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz5xk25fdazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1gl0esx</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are we doing with our blue nails today 🥲 </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl0esx</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1gkyl7m</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green “velvet nails” with a clear thick gel top coat (BIAB) no </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkyl7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1gkue9u</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>are my nails healthy?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkue9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1gkxssi</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WINE 🍷 </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkxssi</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1gkxdxl</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mood: </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkxdxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1gkwfn3</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie Bordeaux - Four Coats </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky9pn9i6p9zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1gkuxyy</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>First time trying Mooncat</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkuxyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1gkuwia</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Zero Degrees magnetized velvet style </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7s6hz3p069zd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1glgc40</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished painting the AHS logo for my nail set! 🥰 </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1t5h6eh6ezd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1glbsiw</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Hypothetical question....</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1glbsiw/hypothetical_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1glb46l</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Needed some cheering up today</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2khel78yczd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1glb3me</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Tried replicating one of those layered resin paintings... with a little twist</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glb3me</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1gl6t0u</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Pastel jumping spiders</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl6t0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1gl5nqx</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">combined with my pc and the sunflowers </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q150zhbtbzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1gl4wjh</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abstract Nails </t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9yvwy4onbzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1gl4iaq</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SOS!!! I need input for my vacation nails! </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gl4iaq</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1gl3l50</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my works </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s26t6ewvdbzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1gl0wax</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Who knows?💎</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9flqbn3ctazd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1gkypqb</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Cheetah nails 🐆🤎🖤</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gkypqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1gky7jp</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Turquoise Christmas sweater nails </t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq61j0s07azd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1gky4xc</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RED Christmas shorties </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gky4xc</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1gktv74</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>A cute halloween design I did this year 👻</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xekazivcs8zd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Nov  8 08:10:28 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_10.xlsx
+++ b/data/collected_data/2024_11_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C862"/>
+  <dimension ref="A1:C1045"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15087,6 +15087,3117 @@
         </is>
       </c>
     </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1gmdj1l</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>My little mermaid nails 🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6qsxk4iwmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1gmd5xd</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Happy Scorpio Season 🦂♏️</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzstqjblrmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1gmcvlg</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dvok White Night Collection </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmcvlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1gmcurv</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dvok White Night Collection </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmcurv</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1gmci6e</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Press Ons I’ve done this year and last </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmci6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1gmcfk7</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Christmas Press Ons I’ve done this year and last</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8v4bcj2imzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1gmbuqa</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Galaxy Nails 💅 </t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8bhpp6abmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1gmbdx7</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to trim these extensions? I’m a noob- not sure what they are called. </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gjenhcz5mzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1gmateg</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Are they blue? Green? Purple? Yes.  Press on!</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmateg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1gmas6l</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Gender reveal nails 🩷💅🏼🩵</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0ea63clzlzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1gmalxk</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>My nail keeps chipping</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lniadxbsxlzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1gm9uwc</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>So close. I still like them, though.</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm9uwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1gm75r7</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Natural nail piercings: looking for advice and opinions!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tejyl1lz0lzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1gm7l9f</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Shein Press-ons</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm7l9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1gm8m9j</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What I asked for (top) and what I got 🥰 by @ xoyanie </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm8m9j</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1gmaafg</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Cat Eyes</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/surh0coiulzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1gma83h</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Cuticles</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gma83h/cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1gma1ax</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fighting for my life with the blooming gel experiment </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ui5ekrytrlzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1gm9tr0</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>What color for a few day beach vacation, then back to winter?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gm9tr0/what_color_for_a_few_day_beach_vacation_then_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1gm9qyw</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Overlay helps me</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6rxrb73plzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1gm9mrp</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Brown nails</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0fk685znlzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1gm89zi</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Disney Nail Set</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm89zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1gm8mf6</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>poker inspired nails ♥️🎱🍒</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm8mf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1gm8x1e</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple and classy! Some of my work </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wd6g193hlzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1gm8qdu</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>seasonal nails✨</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncsf1cydflzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1gm8l38</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Mud Run</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm8l38</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1gm83jg</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for Billie Eilish concert </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bftjusk9lzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1gm7ljt</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Your favorite luxury/long lasting nail polish?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gm7ljt/your_favorite_luxurylong_lasting_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1gm7brz</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I know they are simple... But black never fails... My before and after! </t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sm1bsvc2lzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1gm76j0</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>will a nail salon give gel extensions to a nail biter?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gm76j0/will_a_nail_salon_give_gel_extensions_to_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1gm6jv1</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>November nails 🌸💕💅🏼</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm6jv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1gm5uuz</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Wintery Sparkle Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm5uuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1gm5mlw</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie- Wicked </t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebcfp0wjnkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1gm5gfy</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Cut or keep growing almond? I need a full, I know...</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9g58m7n3mkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1gm5eqy</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s my first time trying press on nails, do they look OK? </t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm5eqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1gm5dji</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t go back 💛 </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0ggqjxelkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1gm4xx5</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Matte nails 🫣</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm4xx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1gm4vvv</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Newest set 🥰</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm4vvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1gm4s6d</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>My new acquisition is something electric ⚡💜</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tbb2943igkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1gm4pq9</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>scooby dooby doo…</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84f908oxfkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1gm4p7z</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>I love my press ons 💅</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wytigatfkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1gm4mvx</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>On a recovery journey after botched gel removal</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kdqo9kafkzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1gm3pqr</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>How do I un-stain my nails?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gm3pqr/how_do_i_unstain_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1gm3em9</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Can't find this product anywhere!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkd5ragg5kzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1gm4cyt</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my clown nails!!!! </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm4cyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1gm47h1</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Had high hopes for these</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4koq1wssbkzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1gm44p0</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Nails for me 😊</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jhaog56bkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1gm3spm</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rate em 🎀 i feel like a fairy </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7abzrpj8kzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1gm3d1d</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue Chrome </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm3d1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1gm3auo</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>fall nails 🍁</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm3auo</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1gm38od</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Decided to try almond for the first time. WDYT</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dy2xv7k54kzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1gm36t2</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Does this shape work with my hands?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm36t2</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1gm2so4</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>2024 Nails</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm2so4</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1gm2gux</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Help!! Can this kind of tips be soaked off with acetone?</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3zwgj9z1yjzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1gm1o8a</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nap nails... Tomorrow is manicure day </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8zy9d91sjzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1gm1eoj</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Fall skittle</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgd5d6d4qjzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1gm0ri9</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Is it too early for winter nails?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma9fse3cljzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1gm15tv</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make press on stay? </t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gm15tv/how_to_make_press_on_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1gm08rk</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Guy starting painting my nails, unsure about brands (and influencer brands)</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gm08rk/guy_starting_painting_my_nails_unsure_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1gm0d0h</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>My favorite set so far🥰</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm0d0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1gm09if</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday set for my sister (only colour/design) </t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm09if</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1gm026w</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Nakey nails</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pni28toyfjzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1glzzwl</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First timer </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bshjuiahfjzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1glzyhe</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Cut or extend?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glzyhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1glz6pj</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>🥰</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jaexvtrh9jzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1glx9bt</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got acrylics for the first time, unable to get them off </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glx9bt/got_acrylics_for_the_first_time_unable_to_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1glwl22</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>How do I fix a scratch on my middle nail and how do I avoid it from happening again?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opx2ygr5qizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1glz1yw</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Leopard print cats eyes nails🤎</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bvb5vsai8jzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1glyyet</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Something New</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/07xmls1s7jzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1glyui9</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>I’m looking forward until my nails will get long enough to repeat this manicure! I loved them so much 🥹🥹</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glyui9</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1glyqb0</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Self done fall vibes! </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7crv5gu36jzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1glypdv</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A nicely done ombré on my big ol hand </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dvkva5x5jzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1glyc9k</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Fresh 🤩</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvixy6d63jzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1gly7b0</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>💀 🧡</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gly7b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1gly554</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are independent nail techs better than salons? </t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gly554/are_independent_nail_techs_better_than_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1glxhnd</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Can’t stop looking at my nails 🥺</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h07nbanuwizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1glwz2j</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>practice makes perfect with frenchies :) proud of where i’ve come</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glwz2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1glwyi1</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>First time trying this caramel brown color 🤎</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/soglhwmvsizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1glwsz9</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>orly gel fx not curing</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1glwsz9/orly_gel_fx_not_curing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1glwms1</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I wanted these colors for autumn vibes! </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glwms1</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1glwjed</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Ohora nail wraps in “Eternal Vow”</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glwjed</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1glwf0k</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Are these bad enough to request a refund?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glwf0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1glwd9l</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>OPI press ons never fail to make me smile.</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tu76x4cjoizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1glw1kc</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>My birthday nails 😊</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg8n8ka5mizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1glvw4z</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>I did my niece's nails, what ya think?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glvw4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1glvtmd</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>black&amp;gold nails🖤🔱</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6kzvbcjkizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1glvjpa</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Learning to do nails at home ! 😊</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86stobsgiizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1glufki</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Trying something new with a splash of old</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35wp9iw7aizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1glu0yd</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Fall Nails are so underrated 😮‍💨😮‍💨</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glu0yd</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1gltedn</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Tips for getting my nails done for the first time?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gltedn/tips_for_getting_my_nails_done_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1gltdsp</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>My nails look at you</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysaxelfd2izd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1glt17g</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>My most recent set is my favorite I’ve ever had 😍</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pktn5qpzhzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1glt05x</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>METALLIC BLUE, nail of the month</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glt05x</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1glsx19</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Can this be fixed?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glsx19</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1glsgle</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Lines on my nail visible 😩</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il6el4z5vhzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1glsheu</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update- Damn you, metal nail file </t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/565huz4cvhzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1glscmk</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>I know they are simple but they look great</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwjmzq48uhzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1glrxnm</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>I asked for skinny almond but I feel like I got stilettos.</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l93ovwz2rhzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1glrw18</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I paid wayyy to much!!! </t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4ge552pqhzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1glrqju</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>First november set 💖</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glrqju</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1gmdmf4</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bee's Knees Lacquer - Ghost Walker </t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmdmf4</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1gmd97u</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Cirque Rose Jelly</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmd97u</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1gmd4lw</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>First Time Trying Chrome (Over Regular Polish)</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvr8r5y3rmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1gm1dnv</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>i want my nails to last longer when they grow in length</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gm1dnv/i_want_my_nails_to_last_longer_when_they_grow_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1glu0nt</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Builder gel question</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glu0nt/builder_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1glu981</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Blooming gel plus normal polish?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glu981/blooming_gel_plus_normal_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1gmcs7e</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Topaz Tears feels appropriate for multiple reasons </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8gtuqwsammzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1gmco5p</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Tried OPI Bubble Bath but I don't think this color fits me. Thoughts ?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vud587zzkmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1gmcgwk</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>When FB marketplace comes through…</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5qfnfniimzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1gmb229</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Atomic Polish - Rubidium?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmb229/atomic_polish_rubidium/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1gm9qqe</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Help with splitting nails!</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vkklnr1plzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1gm97os</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Any Dupes for “Let’s Talk”?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm97os</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1gm90f5</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>fall vibes i was wearing before halloween 🍂🐍</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm90f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1gm8k1w</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Mud Run</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm8k1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1gm844b</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Black Friday Recs?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gm844b/black_friday_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1gm7r0z</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I filled up a Large Priority Mailing box within almost exactly 12 months of being on this sub! </t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/177mazve6lzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1gm7ll6</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First purchase from this brand! Two polishes from BKL The Craft Collection </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm7ll6</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1gm7fhb</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>everyone's nail pictures have brought me joy this week</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm7fhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1gm757n</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lurid - The Crunch of Leaves Underfoot </t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkrkfb5x0lzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1gm6ylb</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>I see those of you with a purple problem, let me show you my red/orange problem…</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zewvia9zkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1gm6fs5</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">why is only the tip on my left thumb nail look matte? </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3u9fc9kukzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1gm69bz</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>I had blue dreams 🌌</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm69bz</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1gm640o</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Mood nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4waou3prkzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1gm5vm3</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Winter Sparkle Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm5vm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1gm5c7f</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Birthday Nails 🤓</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lxfc2xu2lkzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1gm4axb</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Mooncat thoughts?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gm4axb/mooncat_thoughts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1gm3fkn</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>glass blush french manicure</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2ey3tao5kzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1gm335m</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>I wrote you all a Polish Bottles Poem (swipe for part 2)</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm335m</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1gm2erv</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Finally trying Lorraine 🦋</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm2erv</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1gm2dwl</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>little fall floral mani, i love these two shimmers together</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm2dwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1gm1x0r</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Take No Shit. Do No Harm.</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdlf5xsvtjzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1gm1jba</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Polish BF Blurb</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vn3gpizqjzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1gm1ddw</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matching with my nails today! </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ii65zukupjzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1gm16oz</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Y'all were not lying about Starrily magnetics!!!!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i8mut5dgojzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1gm13p2</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>help me narrow down my wishlist (mooncat, ilnp)</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gm13p2/help_me_narrow_down_my_wishlist_mooncat_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1gm0rdw</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Help identifying shade please :)</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8f4tjpbljzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1gm0pye</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>I don’t usually do skittles.</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wy5viwk0ljzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1gm0o3b</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Trying out a thermal</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm0o3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1gm0jfs</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Sparkly Cover Up</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/618msbyljjzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1gm05v1</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Bright green brat nails 💚</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm05v1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1glzb1k</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>In light of recent events I decided to make a November polish rack. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0ovpsefajzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1glytq4</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Need to find petite size press-ons in blank/bulk</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dnos8xs6jzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1glytdf</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Mooncat Emo for Life vs. ILNP Ink?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glytdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1glymna</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>TikTok Viral Nail oil??</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glymna</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1glymme</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Exam Week Nail Polish Haul</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glymme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1glxxge</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Waiting on Midnight Rider to arrive before going blue. For now, Bottled Rage instead.</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glxxge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1glxltf</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>KBShimmer Take It or Leaf It</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glxltf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1glxd8u</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nailtek Recovery kit </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iezd121yvizd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1glwyml</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>A story in 3 acts: tragedy, tragedy strikes again, embrace it as a recognition feature</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glwyml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1glws2g</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sorcery polish </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glws2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1glwogr</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>My nail journey - 2021 to 2023</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glwogr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1glwjsq</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scorpio seduction </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glwjsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1glw2rl</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Can't stop, won't stop buying thermals</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7f8klldmizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1glvtlq</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Was Feeling Sad, So I Did My Nails</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glvtlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1glvbal</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Opinions on Glow in the Dark and Flakie Toppers? (See comment)</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8x7991jgizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1gluyx5</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Favorite Spooky B*tch </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gluyx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1glurxq</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Got The Blues for Red - OPI</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvf87mrqcizd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1gltpg4</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Best hot pink nail polish with no shimmer or glitter? Comment below and add links with photos</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gltpg4/best_hot_pink_nail_polish_with_no_shimmer_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1gltkd6</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Dany Vianna Black Friday?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gltkd6/dany_vianna_black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1glt822</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Feeling a bit dark and shimmery</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/syurull51izd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1glt4hm</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Never too late for blue 💙💛</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wpr2vbtd0izd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1glsqqb</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Peeling Underneath nail?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glsqqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1glsh8n</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Best place to buy stickers?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glsh8n/best_place_to_buy_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1gls8js</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Don't cry bubbles + Insta french</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gls8js</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1gls539</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>As if this week couldn’t get any worse</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0d928i9pshzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1glrjpm</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>well i hope it looks like a fruit?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rf3qmvtnhzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1glrfm4</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I love Frosted metals 💚</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glrfm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1glrb1d</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>DND Nail Lacquer</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glrb1d/dnd_nail_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1glpu05</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>in preparation for black friday, what are your favorite indie/boutique brands?</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glpu05/in_preparation_for_black_friday_what_are_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1glph3u</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>🐾💖 THIS POLISH 💖🐾</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glph3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1glpa0d</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>ILNP Glowstick unmagnetized vs. Flower Child? Photos much appreciated!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glpa0d/ilnp_glowstick_unmagnetized_vs_flower_child/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1glp4e0</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>I love my nails</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yrxjd352hzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1glhcs9</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel polish not sticking </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1glhcs9/gel_polish_not_sticking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1gln3nt</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Planning first Lurid order for the upcoming shop opening </t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efokfou3egzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1gmcr2j</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>This design was on of the most memorable! Still I would prefer flat leaf</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cqm88ogzlmzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1gmckah</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Your thoughts on these nails</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpn5187njmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1gmc9vk</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on Christmas nails that I’ve done this year and last. Slow time right now. Drop me a line tell me what you think. Oh BTW yes I do short nails often LOL 😂 </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxqmoqj5gmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1gm7qt3</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>What material can I use to mix my gel polishes on that's larger than the common resin palettes on amazon? 😊</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gm7qt3/what_material_can_i_use_to_mix_my_gel_polishes_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1gm48fj</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Halloween Nails!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm48fj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1gm37g8</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Unplanned random set (Thumbs on second slide)</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gm37g8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1gm0ryj</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>recreated from @/nail.by.j__ on insta</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s3m9i8gljzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1gltg6y</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>First set of winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgq2ukpv2izd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1glrwkc</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Sliding into Winter</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1glrwkc</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Nov  9 08:09:06 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_10.xlsx
+++ b/data/collected_data/2024_11_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1045"/>
+  <dimension ref="A1:C1232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18198,6 +18198,3185 @@
         </is>
       </c>
     </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1gn56g8</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>My first time doing my own nails and I wanted to try the Korean Glass Nail trend!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2n47h3j0uzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1gn4jum</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Testing out these polygel colors on my daughter</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upucrbxastzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1gn4a3c</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Pink Cat Eye Frenchies</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn4a3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1gn491m</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>VIDEO of the American Horror Story nails! 🥰🫶🏼 For the people that thought they were fake 🤭</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6r57ogalotzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1gn3mxn</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>please help : thin beds , splitting and ultra fragile nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ulpq6l3htzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1gn2tv5</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Candy Apple Red..</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn2tv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1gn4f34</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>BT Art Box Press-ons</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc1i21gqqtzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1gn3or5</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did this! </t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn3or5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1gn2qc3</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Winter blues</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqocidov6tzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1gn2ph7</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Deep maroon nails</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahgyqt0m6tzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1gn25l7</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>My birthday present to myself 🦄</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyyd77aq0tzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1gn1zve</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>I think I did ok. The color I used is OPI gel chocolate moose.</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn1zve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1gn1oqq</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Nail art I did today 😊</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn1oqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1gn1lm5</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tortoise nails </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/932kppq3vszd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1gn15fy</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape looks better on my hands? </t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn15fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1gn0zqf</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Gorgeous set of acrylics I recently had!!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w05chk0pszd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1gn02vh</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>How often do you do your nails and other pressing questions</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gn02vh/how_often_do_you_do_your_nails_and_other_pressing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1gmzoq0</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>A platypus...?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ia1xhcy4cszd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1gn0bjv</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Tried gel extentions and dip powder for the 1st time</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quduk5a8iszd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1gmzy2a</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Told her brown hearts but got red</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkk6yvjkeszd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1gmzkzv</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cant3cy5bszd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1gmzj98</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Slytherin Manicure 🐍🩶💚🖤</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmzj98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1gmz1r8</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Builder Gel Application </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1bhwpz96szd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1gmyxio</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Moving house + social commitments</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hcmp3z65szd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1gmywt7</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Has anyone tried the Limegirl nail kit?</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ugtkaw05szd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1gmxbn4</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Top coat on Glamnetics</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmxbn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1gmtb0g</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>How TF can I get Gel-X w/ tips off at home</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmtb0g/how_tf_can_i_get_gelx_w_tips_off_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1gmytpm</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sog4hdo84szd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1gmw965</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>can a broken nail heal under acrylic?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmw965/can_a_broken_nail_heal_under_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1gmxryj</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>My nails have more curves than my hips</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmxryj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1gmygxg</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would you do this new trend? </t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nivt72m21szd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1gmxu0n</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish stickers </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70wonmodvrzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1gmxmxt</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Help! Which style works for my hands? Oval or square?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmxmxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1gmxmge</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eyes with stickers! </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmxmge</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1gmxlye</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>love them💗🎀🌸</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kiea9a5dtrzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1gmxedx</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A new shape for me </t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjjqkctjrrzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1gmxdfy</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>My current and last set of nails 😊</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmxdfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1gmx5yy</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>learning to cope</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmx5yy/learning_to_cope/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1gmx3c3</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>My finished American Horror Story handpainted season 1 nails! 🥰😭🙏🏼</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pkspswxorzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1gmwx24</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Elegant French Tips with a 3D Bow Accent! 🌸 Thoughts on this classy look? @sarachic.finds</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxuie2r5mrzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1gmww7y</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Got new nails , I love how they came out.🕺</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmww7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1gmw6q9</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Top coat question: orly shining armor</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmw6q9/top_coat_question_orly_shining_armor/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1gmv1ji</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic natural color </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgcf1kt58rzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1gmv0rh</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love a transparent nail! </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yp83ezz7rzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1gmtz8u</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tried a copper chrome! 🧸thoughts? </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmtz8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1gmt9jf</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmt9jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1gmsvvu</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>natural nails</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmsvvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1gmsv7p</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>hand tattoo</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmsv7p/hand_tattoo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1gmsigd</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Subtle and delicate, for the first time with semi-permanent </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amlb8k1hoqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1gmshhv</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Handpainted Autumn nails 🐈 </t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51ji1d1aoqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1gmsa7l</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How's this color? </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycy6auqomqzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1gmrmmk</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Leopard frenchies and cherry nails! 🐆🍒 </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cdtuthohqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1gmriws</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>My After Spooky Season Nails :)</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmriws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1gmrigw</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Fem Nails 💅🏽 still learning 💅🏽🎀</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q971orxtgqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1gmr5jl</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Is it realistic to remove Gel X at home?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmr5jl/is_it_realistic_to_remove_gel_x_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1gmqmwk</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The giant oak tree shedding its leaves in my yard inspired this set. </t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmqmwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1gmqcc2</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little bit of sparkle ✨️ </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzf9pqbo7qzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1gmq72d</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">picture doesn’t do it justice but i swear this is the perfect light pink/nude color. like a soft rosé color.  </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmq72d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1gmq3bb</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails still smell? </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmq3bb/my_nails_still_smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1gmpjbt</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing leopard print nails! </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmpjbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1gmp96t</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Dip with tips, do they look super thick or just me?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmp96t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1gmp7iz</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sabrina Carpenter Nails </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmp7iz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1gmotkg</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye gel polish! </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmotkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1gmosal</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Found the best combo ever for simple galaxy colored nails</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmosal</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1gmomfs</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Looking for nails I can do at home that won't break the bank and will stand up to manual labor</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmomfs/looking_for_nails_i_can_do_at_home_that_wont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1gmohhf</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Could you tell me what product to buy to replicate this nails?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmohhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1gmogrs</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Is it safe to get extensions with a broken nail?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnpc4mgltpzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1gmog1u</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Feeling so feminine 🎀</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jtppz8gtpzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1gmnmso</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>All of my glue has dried out!! How to stop this or substitutes to glue nail tip on?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmnmso/all_of_my_glue_has_dried_out_how_to_stop_this_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1gmn2p5</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Show me your sheer nudes please!</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmn2p5/show_me_your_sheer_nudes_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1gmm1ro</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my nails vs the inspo </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmm1ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1gmmtd0</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>What do you think about this nude color?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0ej6nuehpzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1gmmtbe</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Beginner nail tech. What could I be doing better?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmmtbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1gmmrj2</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>New to doing my own.</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmmrj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1gmmfk4</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Besties who have good nails together stay together </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erzddw2jepzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1gmm0ur</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>would it be rude to bring my own acrylic powder?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmm0ur/would_it_be_rude_to_bring_my_own_acrylic_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1gmlvc8</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>I don’t know how many people like scene nails here, but I was quite proud of this set!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7beqzxzcapzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1gmgyyl</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Beginner using gel here. Finally reached 1.5 weeks without a chip!! I couldn't be more excited to have found what works for me. Maybe my process will help someone else out there just starting out too.</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmgyyl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1gmj8u7</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My latest refill! </t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmj8u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1gmiw3c</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting to think about Christmas nail inspo so had a look back through my Christmas sets from the last couple of years </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmiw3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1gmhexl</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>First Time doing my nails- serious criticism needed, I want to get better and my mom wants me to do this for her 🫣</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmhexl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1gmf03d</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Does anyone know of any fine glitters without any blue specks. I just want pure silver</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmf03d/does_anyone_know_of_any_fine_glitters_without_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1gmkgqk</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Polka dots 😝</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2wwsekhzozd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1gmkczb</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on sizing </t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmkczb/press_on_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1gmjz18</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I'm calling this set "Fun with fairies"</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcq2dt5lvozd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1gmjsv2</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>It’s never too early for Christmas!!</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdaxazt7uozd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1gmj2l6</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Warm fall vibes</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhgoi5s4oozd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1gmj11q</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>New set, who dis</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4r0k03rnozd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1gmi1p2</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Can't apply gel to natural nail??</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmi1p2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1gmhwcs</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Still practising getting there loving the colours.</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzoe9wgudozd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1gmh89m</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Kansas City Chiefs nails!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmh89m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1gmgchk</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Nail day</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtazh7hgxnzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1gmg75z</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Teddy nails 🧸</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmg75z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1gmg3wu</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Help what nail shape suits me?!</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmg3wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1gmg0cc</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>new 🧡</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl1552sctnzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1gmfy7i</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>So pretty 🎀</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmgwxn5ssnzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1gmfxq2</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Nails made by myself</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4utj7h0msnzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1gmf4hv</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Can I put regular polish on gel polish?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gmf4hv/can_i_put_regular_polish_on_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1gn5bfv</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Can’t believe I almost didn’t get this in PPU🩷💚</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1nicnxk72uzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1gn4la2</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Which shops are based in or which ship to the UK?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gn4la2/which_shops_are_based_in_or_which_ship_to_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1gn439z</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What happened </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z1qpi9dmmtzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1gn3p08</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried the horseshoe magnet 🧲 </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ewhlk0nrhtzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1gn3729</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Suggestions/Inspo please for upcoming Euro Christmas Market Trip!</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gn3729/suggestionsinspo_please_for_upcoming_euro/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1gn26qp</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Who's ready for Arcane?? 🦋</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w29qts831tzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1gn1v7u</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best base and top coat? </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gn1v7u/best_base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1gn1rw7</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>You all have lifted me up this week, so I have brought an offering in return. 🙏💙</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/t/ZP8LM3fDx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1gn1d44</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Just a light rant</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gn1d44/just_a_light_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1gn0v2k</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>(Male) with new green nail!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn0v2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1gn0mrd</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>💪</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn0mrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1gn0eff</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This year’s Black Friday sale list from PPU (it’ll be updated as they get more info!) </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://polishpickup.com/pages/indie-black-friday-sales?se_activity_id=157268017303&amp;syclid=csncp5606nis73ccbri0&amp;utm_campaign=Indie+Black+Friday+Sales+List+2024_157268017303&amp;utm_medium=email&amp;utm_source=shopify_email</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1gn07bk</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>magical girl vibes 💖🌙</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jk05vsa2gszd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1gmylwt</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eerie Embers of Salem for this weeks mani….it just seems to fit right now. </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmylwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1gmybgb</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do nail salon manicures not smell? </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmybgb/why_do_nail_salon_manicures_not_smell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1gmxamx</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>For your viewing pleasure</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lqxdlw5nqrzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1gmxagr</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Rothko Red</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmxagr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1gmwkxp</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Dupe for Emily de Molly Double Cross?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmwkxp/dupe_for_emily_de_molly_double_cross/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1gmwcdq</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Incredible</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jnthooqirzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1gmw0bp</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Blue 💙</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6pdyapbzfrzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1gmvn0c</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>A little neutral rose gold sparkle</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0308pmezcrzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1gmvgxj</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Saw the purples and reds, I’ll bring the blues…</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbtlzutjbrzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1gmv1w6</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>What 3 weeks of wear looks like (aka I’m too lazy to do my nails)</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmv1w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1gmueos</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>got my first bottle of indie polish since getting back into this as a hobby!!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24vfp8453rzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1gmtx25</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Working on my masters degree, working on my nails..</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmtx25</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1gmthxd</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>🍂🍁🍂 Crunchy Yellow Leaves 🍂🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmthxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1gmtev3</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Is my first time posting here what do you think ♥️</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmtev3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1gmt83v</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you like Them Apples? 🍎 🍏 </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmt83v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1gmt2b0</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>got a nude mani for the first time &amp; pleasantly surprised by how much I like it</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmt2b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1gmsynd</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Psilo-sibling comparison  (from @clionadhcosmetics on insta)</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmsynd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1gmsgmw</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>So annoyed I could cry… What I wanted vs what I got</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmsgmw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1gms1ik</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Fall party nails</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gms1ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1gmrtch</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Psilocybin is restocked!!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu7hm1d3jqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1gmrkit</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I wanted to join in on the blue nail trend. </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmrkit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1gmr6g7</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>First time trying Holo Taco and I’m SHOOK at how ✨ stunning ✨ it is</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmr6g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1gmqslt</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>ilnp moonlit</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k8s6ddmwaqzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1gmqklk</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Favorite holiday polishes?</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmqklk/favorite_holiday_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1gmqdxj</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>What’s your favorite indie polish brand?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmqdxj/whats_your_favorite_indie_polish_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1gmq5qp</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Something sweet to end the week</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmq5qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1gmq1gt</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my coping manicure </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8it4wyme5qzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1gmpkmz</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>ABCs of polish! X is for XXVZ Nails</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3jjx5hx1qzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1gmphzy</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>When you can't decide which color to paint, so you choose all of them 🥺✨️</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yiuhby691qzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1gmp9da</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Careful, I Bite 🩸✨</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmp9da</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1gmp86p</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Put this on for autumn and I am obsessed with how sparkly it is. </t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmp86p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1gmp75g</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">one nail is looking weird &amp; dermatologist said it’s “normal" but i'm not convinced </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmp75g/one_nail_is_looking_weird_dermatologist_said_its/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1gmp62z</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling Blue 💙😔 </t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmp62z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1gmoms3</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>The name of this polish is rather accurate to my mood given the current events in the world…</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/juqyp0qsupzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1gmok9s</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Decided to treat myself after recent events</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97wgidtaupzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1gmnvhl</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>'Two' polishes in one tiny bottle!  😀🌸💜</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/nov-2024-mini-polish-Ho1eEyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1gmnjuj</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Me spinning around in circles in my front yard while recoding my nails, so I can show you how shifty this polish is in different lighting</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bdw3vx2umpzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1gmn89m</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Glowy to the next level of</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmn89m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1gmn82e</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Dupe nail polish for this mooncat.</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mijmg70hkpzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1gmn7n1</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>LSD is wild</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yufuymndkpzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1gmn0lj</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Lmao 💀</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmn0lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1gmmh7q</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Superclusterfck</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmmh7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1gmmas1</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Mooncat longevity issues</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmmas1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1gmm62t</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Borealis Scenery</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hkz0wlikcpzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1gmm4iv</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freezer Burned Queen Bee </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmm4iv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1gmljgr</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Synchronous- Envy Lacquer</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/23set31s7pzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1gmlcbt</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>OPIxWicked: Witch O’clock &amp; Oz-mazing</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmlcbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1gml502</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for PFD - quite literally dead inside </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p97rk9vp4pzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1gmk6l1</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Sharing my current wishlist for Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmk6l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1gmk4pa</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Rainbow connection</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmk4pa/rainbow_connection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1gmj8wk</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Hypnotic Polish Mooncat magnetic wand</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmj8wk/hypnotic_polish_mooncat_magnetic_wand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1gmj6rr</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>My women’s suffrage nails</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmj6rr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1gmivqh</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Looking for a Tiger’s Eye stone color ✨</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmivqh/looking_for_a_tigers_eye_stone_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1gmhzy3</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧸Teddy Manicure inspired ✨️ </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmhzy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1gmhdj4</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Mani Mag Velvet Nails</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jmgl8l6q8ozd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1gmh3de</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>A light in the darkness</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmh3de</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1gmg40k</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>I absolutely adore this colour 🥀</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmg40k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1gmegfh</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your absolute favorite top 3 polishes? </t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gmegfh/what_are_your_absolute_favorite_top_3_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1gmdqqg</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Feeling blue</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w8r6cfbzmzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1gmzpay</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Koi Fish Nails</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmzpay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1gmzlj2</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>New to Nail Art</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u4z5qibbszd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1gmz91y</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Do you like this?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u9eyue48szd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1gmx2t2</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>My finished American Horror Story handpainted season 1 nails! 🥰😭🙏🏼</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wyysmptorzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1gmwkei</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>After all the positive feedback on my last post: here's the rest of the hand</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmwkei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1gmwejx</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>I'm so happy how they turned out! ✨️</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmwejx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1gmsywo</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not usually a red fan… </t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw8yjnmyrqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1gmrn6o</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Leopard frenchies and cherry nails! 🐆🍒</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/satxvjgshqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1gmri0z</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Handpainted Autumn nails</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ngxdfpqgqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1gmr2vj</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Pop punk with Sanrio &amp; domo &lt;3</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc498qjfdqzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1gmp5ha</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Little koi fish ponds</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmp5ha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1gmo735</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Very vibrant and/or glittery cat-eye polishes - recs</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gmo735/very_vibrant_andor_glittery_cateye_polishes_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1gmo4ao</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Playing with Christmas ideas </t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmo4ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1gml7p9</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>cozy fall nails. Reminds me of hot chocolate or cocoa with marshmallows</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gml7p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1gmk67o</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute Halloween 🎃 Nailart by my daughter ❤️ </t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmk67o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1gmjkte</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>My attempt at the grinch nails - what do you think? 💕</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwq873odsozd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1gmh5n7</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>A candy manicure that you can rate;)</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmh5n7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Nov 10 08:09:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_10.xlsx
+++ b/data/collected_data/2024_11_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1232"/>
+  <dimension ref="A1:C1411"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21377,6 +21377,3049 @@
         </is>
       </c>
     </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1gnvqnl</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnvqnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1gnvomm</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>First time doing my own gel nails!</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mmmqlog510e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1gnvhk6</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm freaking obsessed with polygel. </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8957soft210e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1gnuvkj</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>I love this Christmas design 💗</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ormyda2v00e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1gnuqne</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At home gel manicure kit recommendations </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnuqne/at_home_gel_manicure_kit_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1gnumoe</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Had a 90's themed party so I painted my nails accordingly!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ng0sf89zr00e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1gnsxvm</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Help, how long should Jello Jello One Kill base last?</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnsxvm/help_how_long_should_jello_jello_one_kill_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1gnu579</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Fresh pedi</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfvkdo90m00e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1gnt1ja</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Why do bad things happen to good people? I was going to give them some TLC tomorrow!</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1iy39nbq900e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1gnsupu</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel x nails first time </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnsupu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1gnsquf</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>November nails to match the mood/vibe 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id54smgm600e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1gnsbun</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Is there an app I can use to create my nail ideas before actually making them?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnsbun/is_there_an_app_i_can_use_to_create_my_nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1gnrsz8</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Go for Gold!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9x0gbsrwzzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1gnrrlv</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>this gel-x set i did on myself was fun 🤍(please excuse the dark photo, but my ass is in bed)</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j65uqjtdwzzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1gns721</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>These are her natural nails! 😍</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rba5r6ps000e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1gnrti2</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Is this normal grow out for a week? Does it look bad? I need these to last 2 more weeks</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnrti2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1gnrj9r</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Can I use acetone on UV cured acrylics?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnrj9r/can_i_use_acetone_on_uv_cured_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1gnr0u6</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>todays long gel x set 🤎</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3u7o1wwozzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1gnr0qi</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails a size too small, does this look okay? </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnr0qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1gnqi2p</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Let’s talk about this color 😍</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kpae12qjzzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1gnqq9c</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Halloween nails 🕸️</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to927sgzlzzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1gnqo13</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Gel X</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v97xq3ddlzzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1gnqh5b</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>🤎🤍</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnqh5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1gnqak7</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">still new at this! </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnqak7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1gnpf8x</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Wanted to show them off</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grrov2v59zzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1gnp5qf</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>these press ons are perfect!!</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q26wyi6p6zzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1gnp365</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Is there a comprehensive kit for DIY press ons?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnp365/is_there_a_comprehensive_kit_for_diy_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1gnoa37</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>My ideal nails</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnc39j6nyyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1gno4lp</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Green 💚💚</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl4b7lu9xyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1gno2ca</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic red for Christmas tree decorating </t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drzetexpwyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1gnns06</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t xml:space="preserve">10 Years Later ✨💍 </t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnns06</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1gnm6tr</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Nails inspired by Chappell Roan's VMAs looks. Swipe through to see some of the reimagined design elements &amp; my inspo board🗡️⛓️</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnm6tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1gnmaoy</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Is this a good nail dehydrator for press ons? If not any recommendations?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nnsesqahyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1gnnk34</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>First time with glue on nails, im worried they look to big for my fingers? Half eaten banana for scale?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a027a8p9syzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1gnnf4w</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Celestial 🌠</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s01aykb0ryzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1gnm7zn</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Funky in Fall ⭐️</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oj3iznxmgyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1gnm6yu</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Just playing around with mismatched art</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnm6yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1gnlqdk</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Why do only men do my nails at salons?</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnlqdk/why_do_only_men_do_my_nails_at_salons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1gnlfdr</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best stuff to practice on? </t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnlfdr/best_stuff_to_practice_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1gnl7jm</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyn574i58yzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1gnl3hx</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh gel mani in reds &amp; pinks! I took my acrylics off in May and my nails are finally growing long &amp; strong again ❤️ 😍 </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnl3hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1gnk720</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>What do I do next?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rhtp5dtzxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1gnkw9e</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Short and sweet</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnkw9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1gnkl0i</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips for using gold leaf? </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnkl0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1gnhdhb</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Easy to remove?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnhdhb/easy_to_remove/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1gnjw8d</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - What You Water Grows 💦🪴</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnjw8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1gnivu3</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>I'm in love</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnivu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1gnigiz</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Long nails don’t care</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/viuouy6jlxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1gniczh</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>My attempt at The Grinch nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22tnp4sqkxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1gni8jh</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do my nails give fall vibes 🍂? </t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/26x1z9hpjxzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1gni514</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Recent Gel Sets 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gni514</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1gni17l</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Dark green 🌳💚</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gni17l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1gnhv85</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>in love with my new set!</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sd24h9qgxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1gnhttz</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My regular lady wasn’t there to jazz them up so I went simple for Thanksgiving </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c1l1kkfgxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1gnhmns</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>had to change colors</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjfrisftexzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1gnhioj</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>I love love LOVE nail sets with the charms/gems secured with resin!</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xevqmoevdxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1gnb2mg</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>How do I stop nail from splitting like this?</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itef9gx7xvzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1gnh5zi</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnh5zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1gngqst</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Nude cateye almond nails 😍</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gngqst</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1gngge8</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gngge8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1gngdso</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Pink Nails 🍬 </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggepfs9r4xzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1gnfasp</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>What full cover tips would fully fit my nails?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah0wg4m4wwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1gng7tz</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>folding laundry + new neutral set ✨</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynlpuuwf3xzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1gng74e</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>November’s nails, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2wc3nda3xzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1gnfyet</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>blue glitter nails 💙</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnfyet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1gnfe1x</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dropping hints 💕 </t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjxkfx9vwwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1gnf9nc</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>November nails! 🍎</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnf9nc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1gnex3y</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>why is it everytime i ask for something other then just painted plain they fuck it up :(</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnex3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1gncrj7</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's the best way for me to get my nails done without damaging them or their health ? </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gncrj7/whats_the_best_way_for_me_to_get_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1gne5d6</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Why are my nails like this?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gne5d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1gnekhh</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>New nails!!!</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhfkqofaqwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1gneijb</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Basic</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7llho06wpwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1gn9fsz</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Can the nail bed grow?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn9fsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1gne4d9</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>I like my blue nails</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0ki13krmwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1gndj0j</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Purple and green cat eye 💜💚</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kfei5teuhwzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1gnctq6</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Jumping on the leopard print trend 😺</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/332324o5cwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1gnchnl</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>First time ever doing gel nails. Hoping they won't lift 🙏</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35flkhzd9wzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1gnbt7i</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Primaverales 💐</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wagp1ddr3wzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1gnbnwa</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need some help relating to polygel </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gnbnwa/need_some_help_relating_to_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1gnb50t</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Cadillaquer- Basil + Orly- Glow In The Dark</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnb50t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1gnaxqx</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Daughter did my Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2cheqqyvvzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1gnat52</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Lisbon Wants Moor OPI</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihz4nsusuvzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1gnasdm</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">lastest manicure done by my nail tech, milky white base with black french tips </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnasdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1gna83u</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Some sets done by me🥰</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gna83u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1gn9y6o</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail art hat </t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w3n1ueqmvzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1gn9uvi</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>What do you think of my rainbow nails? 🌈✨</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aclz25folvzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1gn9psh</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>What do you think about my nails?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn9psh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1gn95qr</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>diy pink heart nails ♡</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m4w2p07sevzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1gn8bgn</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>What would you call this design? It’s giving me LOTR vibes🧝‍♀️</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzv6x05d5vzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1gn7t3x</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Fairycore 🧚</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/orsv6g44zuzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1gn6e7m</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Ideas for classy Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gn6e7m/ideas_for_classy_christmas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1gn63yi</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Prestigious purple</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn63yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1gn5zf1</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>This week red will be my color (:</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrckx3yyauzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1gnu1o0</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Nail swatches!</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khmztuoxk00e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1gnt93x</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recs for similar nail toppers? </t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnt93x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1gnsytp</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>KB Shimmer Smooth Moves dulls reflective glitter?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnsytp/kb_shimmer_smooth_moves_dulls_reflective_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1gnsoxb</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Black pigment streaks (?)</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnsoxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1gns0nb</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Dupe request: PFD Eternal Glow</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gns0nb/dupe_request_pfd_eternal_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1gnr7cw</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Booked a Massage After This Happened to Help Cope</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9azt6zfpqzzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1gnpmta</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>I used some interesting inspo</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnpmta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1gnplej</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Which ILNP shade is closest to “Paradise”?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaq646osazzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1gnpd47</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Deep dive: Mixing my own glow in the dark nail polish</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnpd47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1gno9uc</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using magnetic polish </t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gno9uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1gno3ni</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>2nd try at nail art!</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwtyxiq1xyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1gno3e1</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>is gel even worth it?</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gno3e1/is_gel_even_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1gnnu0m</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Dupe for Chanel Paradoxal</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnnu0m/dupe_for_chanel_paradoxal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1gnn9cz</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Canadian Lacqueristas - Do you know if Harlow and Co does a Black Friday sale?</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnn9cz/canadian_lacqueristas_do_you_know_if_harlow_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1gnn7b6</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>kbshimmer magnetic troubles</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnn7b6/kbshimmer_magnetic_troubles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1gnmzhp</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Unhinged Request...help me find this polish?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfx9vub7nyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1gnmtam</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>elegant. ghostly. lovely. everything i have ever wanted &amp; more</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ln7uekplyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1gnmont</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Sparkly fall nails ✨️</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnmont</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1gnmis8</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>I often think that the night is more alive and more richly colored than the day - Vincent van Gogh</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnmis8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1gnmfvq</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted something bright </t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/034h6z5eiyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1gnmak2</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Having fun with stripes and holo</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnmak2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1gnm0lh</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Cannot stop staring. Beautiful rainbow holo</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnm0lh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1gnlu6u</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Screw it, I'm living in Lala Land </t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be6b8j2ddyzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1gnl8re</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>First lurid order  - is this too much purple?</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djww6mef8yzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1gnkgsn</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Another Psilocybin Post</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4xehjyv1yzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1gnkdnj</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Velvet jewels courtesy of Starrily</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnkdnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1gnk8p5</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I prefer an action shot myself </t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tbmnitylzxzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1gnk4b3</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do I do now that I’ve over filled my nails? </t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnk4b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1gnjzvk</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>BCB Lacquers - What You Water Grows 💦🪴</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnjzvk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1gnjs43</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>So Captivating</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnjs43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1gnjatp</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Mourning colors</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uom2o7mfsxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1gnj7xi</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What kind of leaf or plant would you call this general design? </t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnj7xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1gnj4d0</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Simple pearl for the indecisive</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnj4d0/simple_pearl_for_the_indecisive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1gnebl7</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnebl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1gni1dg</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Fav brands?</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gni1dg/fav_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1gniiou</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Took off the blue, put on Indomitable</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gniiou</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1gnhn7d</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>How many polishes do you have?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnhn7d/how_many_polishes_do_you_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1gnhm0x</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will a thermal work over a regular polish? </t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnhm0x/will_a_thermal_work_over_a_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1gnhg8o</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Thin French manicure</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqikbf4cdxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1gnh3la</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>November nails so far</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnh3la</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1gnguq5</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Teal vines</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnguq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1gngrlk</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Back with more Welcome to the Witching Hour ✨️🔮</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gngrlk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1gngf8v</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>My mani pick for this week’s Lurid launch!</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gngf8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1gng5hz</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Got lucky on FB Marketplace and found an ex-swatcher doing a destash</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gng5hz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1gng0ec</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>It looked different in the bottle</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gng0ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1gnfx89</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Does anyone use GlitterUnique quick dry top coat?  Opinions please</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnfx89/does_anyone_use_glitterunique_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1gnfv2z</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Giving off Fall moody vibes 🌧</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k4wp3uo0xzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1gnfmb1</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>What are your favorite most shiftiest polishes?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnfmb1/what_are_your_favorite_most_shiftiest_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1gnfl9j</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">getting my hair done so mine as well show the nail color of the moment </t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z59wflthywzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1gnez6v</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>What should my manicure be for NWSA?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gnez6v/what_should_my_manicure_be_for_nwsa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1gnet9k</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>My most hated polished and the comments I have received when I use them</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnet9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1gnep39</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pleasantly Surprised </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnep39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1gnehl5</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>BF list. Talk me out of polishes that you found disappointing!</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vljoz8topwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1gneayx</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Racing Nails for my boyfriend's birthday</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gneayx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1gne7fb</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>My nails and my mug!</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnqdledgnwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1gne6kq</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails and Essie “Rocky Rose” </t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20uvogu8nwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1gndy4a</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hard Candy "Sky" </t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/664556talwzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1gndoyk</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Looking for thermal polishes that go from clear to a color?</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gndoyk/looking_for_thermal_polishes_that_go_from_clear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1gndfrg</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>The weekly dilemma of choosing a color(s)</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh6hm6j6hwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1gnderm</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Artemis by Live Love Polish</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uuu7h39ygwzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1gnd24s</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>at least i have space nails 🌌✨</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnd24s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1gnc2wg</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>ILNP clover!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnc2wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1gnbu6j</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coffee Nails? </t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnbu6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1gnbq9z</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>such a stunning color 😍</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnbq9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1gnb5ro</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Cadillaquer - Basil + ORLY - Glow In The Dark</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnb5ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1gna54o</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>What polishes would in the Lacquerista Hall of Fame?</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gna54o/what_polishes_would_in_the_lacquerista_hall_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1gn97xf</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Vintage Blue (History)</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5sup4ncefvzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1gn965x</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made this using nail polish :) </t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n0bg4ntwevzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1gn8oxh</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>My past manis</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn8oxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1gmuo65</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Mooncat The Glory of Innocence</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gmuo65</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1gn7md7</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Suuuuper shifty magnetic from I Scream Nails</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gn7md7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1gnuff8</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Wife’s nails</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unlxrjdgp00e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1gnu65i</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Nail art novice</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnu65i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1gnsao3</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssti6szu100e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1gnr1b4</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My little garden </t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnr1b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1gnnl7m</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Green 💚💚💚</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hazzwdnjsyzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1gnm88a</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Having fun with black and holo. Threw in some crackle and glitter for good measure</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnm88a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1gnlxke</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Nails Inspired by Chappell's VMAs looks- swipe to see some of the elements I pulled from &amp; my inspo board🖤</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnlxke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1gnk68j</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Dusty Thunder Ascon Scale Nails</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnk68j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1gnik7u</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>I painted a beluga on my nails</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unswken7mxzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1gni1mn</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Don't touch it's art 🎨 ! by : @sarachic.finds</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t23yvxo0ixzd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1gnhnee</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>November nails</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gnhnee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1gnflrz</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this 💕 </t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh9sng0mywzd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1gndwuv</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Simple disney “Lilo &amp; Angel” nails 💕</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlipofk2lwzd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1gndmb4</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>I tried creating some AI nails in real life☁️☁️☁️</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gndmb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1gnbsyr</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>my beautiful yellow nails</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gnbsyr/my_beautiful_yellow_nails/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>